<commit_message>
Updated Map, Board, and Turndown Chart
Map more closely matches classic Pacman board
</commit_message>
<xml_diff>
--- a/2017SP_Burndown-Chart-Pacman.xlsx
+++ b/2017SP_Burndown-Chart-Pacman.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcowen/Dropbox/LMSC-281/Week 13/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcowen/GitHub-Berklee/LMSC281_PacMan-Clone-Update/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockStructure="1"/>
@@ -1329,8 +1329,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="839177632"/>
-        <c:axId val="839166816"/>
+        <c:axId val="684426208"/>
+        <c:axId val="684417520"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1378,13 +1378,13 @@
                   <c:v>32.18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.35</c:v>
+                  <c:v>30.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.52</c:v>
+                  <c:v>29.02</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.69</c:v>
+                  <c:v>27.44</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.0</c:v>
@@ -1689,11 +1689,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="839177632"/>
-        <c:axId val="839166816"/>
+        <c:axId val="684426208"/>
+        <c:axId val="684417520"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="839166816"/>
+        <c:axId val="684417520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1748,12 +1748,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="839177632"/>
+        <c:crossAx val="684426208"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:dateAx>
-        <c:axId val="839177632"/>
+        <c:axId val="684426208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1780,7 +1780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="839166816"/>
+        <c:crossAx val="684417520"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1828,7 +1828,7 @@
         <xdr:cNvPr id="2" name="shape">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CA6FF4D-82E2-477E-8E4C-685A2FFBD528}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3CA6FF4D-82E2-477E-8E4C-685A2FFBD528}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2148,7 +2148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DN110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -6743,7 +6743,7 @@
   <dimension ref="A1:DB138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="59.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7079,15 +7079,15 @@
       <c r="D2"/>
       <c r="G2" s="20" t="str">
         <f ca="1">IF(G$37=$B$35,"Today",IF(G$37&lt;$B$35,"P","F"))</f>
-        <v>Today</v>
+        <v>P</v>
       </c>
       <c r="H2" s="20" t="str">
         <f t="shared" ref="H2:AM2" ca="1" si="0">IF(AND($B$35&gt;G$37,$B$35&lt;=H$37),"Today",IF(H$37&lt;$B$35,"P","F"))</f>
-        <v>F</v>
+        <v>P</v>
       </c>
       <c r="I2" s="20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>F</v>
+        <v>Today</v>
       </c>
       <c r="J2" s="20" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -7905,11 +7905,11 @@
       </c>
       <c r="D4" s="27">
         <f>SUM($D$38:$D$138)</f>
-        <v>33.35</v>
+        <v>30.6</v>
       </c>
       <c r="E4" s="27">
         <f>(C4-D4)/B1</f>
-        <v>-1.1700000000000017</v>
+        <v>1.5799999999999983</v>
       </c>
       <c r="G4" s="20">
         <f t="shared" ref="G4:AL4" si="3">IF(G36&lt;&gt;"F",SUM(G$38:G$138),"")</f>
@@ -8320,7 +8320,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="28">
         <f ca="1">C4-(E4*(Setup!$B$6-1))</f>
-        <v>35.690000000000005</v>
+        <v>27.440000000000005</v>
       </c>
       <c r="E5" s="27"/>
       <c r="G5" s="29">
@@ -8329,15 +8329,15 @@
       </c>
       <c r="H5" s="29">
         <f t="shared" ca="1" si="6"/>
-        <v>33.35</v>
+        <v>30.6</v>
       </c>
       <c r="I5" s="29">
         <f t="shared" ca="1" si="6"/>
-        <v>34.520000000000003</v>
+        <v>29.020000000000003</v>
       </c>
       <c r="J5" s="29">
         <f t="shared" ca="1" si="6"/>
-        <v>35.690000000000005</v>
+        <v>27.440000000000005</v>
       </c>
       <c r="K5" s="29" t="str">
         <f t="shared" ca="1" si="6"/>
@@ -9283,11 +9283,11 @@
       </c>
       <c r="D9" s="31">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="27">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="20">
         <f t="shared" si="12"/>
@@ -11393,11 +11393,11 @@
       </c>
       <c r="D14" s="31">
         <f t="shared" si="10"/>
-        <v>1.75</v>
+        <v>0</v>
       </c>
       <c r="E14" s="27">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="G14" s="20">
         <f t="shared" si="12"/>
@@ -17840,11 +17840,11 @@
       </c>
       <c r="D31" s="31">
         <f>SUMIF($B$38:$B$138,$B31,$D$38:$D$138)</f>
-        <v>33.35</v>
+        <v>30.6</v>
       </c>
       <c r="E31" s="27">
         <f>(C31-D31)/B$1</f>
-        <v>-1.1700000000000017</v>
+        <v>1.5799999999999983</v>
       </c>
       <c r="G31" s="20">
         <f t="shared" ref="G31:P33" si="32">SUMIF($B$38:$B$138,$B31,G$38:G$138)</f>
@@ -19096,19 +19096,19 @@
       </c>
       <c r="B35" s="25">
         <f ca="1">TODAY()</f>
-        <v>42853</v>
+        <v>42855</v>
       </c>
       <c r="G35" s="20" t="str">
         <f ca="1">IF(G$37=$B$35,"Today",IF(G$37&lt;$B$35,"P","F"))</f>
-        <v>Today</v>
+        <v>P</v>
       </c>
       <c r="H35" s="20" t="str">
         <f t="shared" ref="H35:AM35" ca="1" si="42">IF(AND($B$35&gt;G$37,$B$35&lt;=H$37),"Today",IF(H$37&lt;$B$35,"P","F"))</f>
-        <v>F</v>
+        <v>P</v>
       </c>
       <c r="I35" s="20" t="str">
         <f t="shared" ca="1" si="42"/>
-        <v>F</v>
+        <v>Today</v>
       </c>
       <c r="J35" s="20" t="str">
         <f t="shared" ca="1" si="42"/>
@@ -21601,8 +21601,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="31">
-        <f t="shared" ref="D41:D69" si="55">DB41</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41" s="38"/>
       <c r="F41" s="39" t="s">
@@ -21613,399 +21612,399 @@
         <v>1</v>
       </c>
       <c r="H41" s="20">
-        <f t="shared" ref="H41:AM41" si="56">G41</f>
+        <f t="shared" ref="H41:AM41" si="55">G41</f>
         <v>1</v>
       </c>
       <c r="I41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="J41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="K41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="L41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="M41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="N41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="O41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="P41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="Q41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="R41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="S41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="T41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="U41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="V41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="W41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="X41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="Y41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="Z41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AA41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AB41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AC41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AD41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AE41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AF41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AG41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AH41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AI41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AJ41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AK41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AL41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AM41" s="20">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AN41" s="20">
+        <f t="shared" ref="AN41:BS41" si="56">AM41</f>
+        <v>1</v>
+      </c>
+      <c r="AO41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="J41" s="20">
+      <c r="AP41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="K41" s="20">
+      <c r="AQ41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="L41" s="20">
+      <c r="AR41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="M41" s="20">
+      <c r="AS41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="N41" s="20">
+      <c r="AT41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="O41" s="20">
+      <c r="AU41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="P41" s="20">
+      <c r="AV41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="Q41" s="20">
+      <c r="AW41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="R41" s="20">
+      <c r="AX41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="S41" s="20">
+      <c r="AY41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="T41" s="20">
+      <c r="AZ41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="U41" s="20">
+      <c r="BA41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="V41" s="20">
+      <c r="BB41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="W41" s="20">
+      <c r="BC41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="X41" s="20">
+      <c r="BD41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="Y41" s="20">
+      <c r="BE41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="Z41" s="20">
+      <c r="BF41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AA41" s="20">
+      <c r="BG41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AB41" s="20">
+      <c r="BH41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AC41" s="20">
+      <c r="BI41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AD41" s="20">
+      <c r="BJ41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AE41" s="20">
+      <c r="BK41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AF41" s="20">
+      <c r="BL41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AG41" s="20">
+      <c r="BM41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AH41" s="20">
+      <c r="BN41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AI41" s="20">
+      <c r="BO41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AJ41" s="20">
+      <c r="BP41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AK41" s="20">
+      <c r="BQ41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AL41" s="20">
+      <c r="BR41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AM41" s="20">
+      <c r="BS41" s="20">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AN41" s="20">
-        <f t="shared" ref="AN41:BS41" si="57">AM41</f>
-        <v>1</v>
-      </c>
-      <c r="AO41" s="20">
+      <c r="BT41" s="20">
+        <f t="shared" ref="BT41:DB41" si="57">BS41</f>
+        <v>1</v>
+      </c>
+      <c r="BU41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="AP41" s="20">
+      <c r="BV41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="AQ41" s="20">
+      <c r="BW41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="AR41" s="20">
+      <c r="BX41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="AS41" s="20">
+      <c r="BY41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="AT41" s="20">
+      <c r="BZ41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="AU41" s="20">
+      <c r="CA41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="AV41" s="20">
+      <c r="CB41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="AW41" s="20">
+      <c r="CC41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="AX41" s="20">
+      <c r="CD41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="AY41" s="20">
+      <c r="CE41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="AZ41" s="20">
+      <c r="CF41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BA41" s="20">
+      <c r="CG41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BB41" s="20">
+      <c r="CH41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BC41" s="20">
+      <c r="CI41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BD41" s="20">
+      <c r="CJ41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BE41" s="20">
+      <c r="CK41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BF41" s="20">
+      <c r="CL41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BG41" s="20">
+      <c r="CM41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BH41" s="20">
+      <c r="CN41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BI41" s="20">
+      <c r="CO41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BJ41" s="20">
+      <c r="CP41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BK41" s="20">
+      <c r="CQ41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BL41" s="20">
+      <c r="CR41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BM41" s="20">
+      <c r="CS41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BN41" s="20">
+      <c r="CT41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BO41" s="20">
+      <c r="CU41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BP41" s="20">
+      <c r="CV41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BQ41" s="20">
+      <c r="CW41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BR41" s="20">
+      <c r="CX41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BS41" s="20">
+      <c r="CY41" s="20">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="BT41" s="20">
-        <f t="shared" ref="BT41:DB41" si="58">BS41</f>
-        <v>1</v>
-      </c>
-      <c r="BU41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="BV41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="BW41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="BX41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="BY41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="BZ41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CA41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CB41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CC41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CD41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CE41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CF41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CG41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CH41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CI41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CJ41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CK41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CL41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CM41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CN41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CO41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CP41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CQ41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CR41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CS41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CT41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CU41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CV41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CW41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CX41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
-      <c r="CY41" s="20">
-        <f t="shared" si="58"/>
-        <v>1</v>
-      </c>
       <c r="CZ41" s="20">
-        <f t="shared" si="58"/>
+        <f t="shared" si="57"/>
         <v>1</v>
       </c>
       <c r="DA41" s="20">
-        <f t="shared" si="58"/>
+        <f t="shared" si="57"/>
         <v>1</v>
       </c>
       <c r="DB41" s="20">
-        <f t="shared" si="58"/>
+        <f t="shared" si="57"/>
         <v>1</v>
       </c>
     </row>
@@ -22022,7 +22021,7 @@
         <v>2</v>
       </c>
       <c r="D42" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" ref="D41:D69" si="58">DB42</f>
         <v>2</v>
       </c>
       <c r="E42" s="38"/>
@@ -22443,7 +22442,7 @@
         <v>2</v>
       </c>
       <c r="D43" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>2</v>
       </c>
       <c r="E43" s="38"/>
@@ -22864,7 +22863,7 @@
         <v>1</v>
       </c>
       <c r="D44" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="E44" s="38"/>
@@ -23285,7 +23284,7 @@
         <v>2</v>
       </c>
       <c r="D45" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>2</v>
       </c>
       <c r="E45" s="38"/>
@@ -23706,7 +23705,7 @@
         <v>2</v>
       </c>
       <c r="D46" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>2</v>
       </c>
       <c r="E46" s="38"/>
@@ -24127,7 +24126,7 @@
         <v>2</v>
       </c>
       <c r="D47" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>2</v>
       </c>
       <c r="E47" s="38"/>
@@ -24548,7 +24547,7 @@
         <v>1</v>
       </c>
       <c r="D48" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="E48" s="38"/>
@@ -24969,7 +24968,7 @@
         <v>1</v>
       </c>
       <c r="D49" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="E49" s="38"/>
@@ -25390,7 +25389,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="E50" s="38"/>
@@ -25811,7 +25810,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="E51" s="38"/>
@@ -26232,7 +26231,7 @@
         <v>2</v>
       </c>
       <c r="D52" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>2</v>
       </c>
       <c r="E52" s="38"/>
@@ -26653,7 +26652,7 @@
         <v>2</v>
       </c>
       <c r="D53" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>2</v>
       </c>
       <c r="E53" s="38"/>
@@ -27074,7 +27073,7 @@
         <v>2</v>
       </c>
       <c r="D54" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>2</v>
       </c>
       <c r="E54" s="38"/>
@@ -27495,8 +27494,7 @@
         <v>0.1</v>
       </c>
       <c r="D55" s="31">
-        <f t="shared" si="55"/>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E55" s="38"/>
       <c r="F55" s="39" t="s">
@@ -27916,8 +27914,7 @@
         <v>0.5</v>
       </c>
       <c r="D56" s="31">
-        <f t="shared" si="55"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E56" s="38"/>
       <c r="F56" s="39" t="s">
@@ -28337,8 +28334,7 @@
         <v>0.15</v>
       </c>
       <c r="D57" s="31">
-        <f t="shared" si="55"/>
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E57" s="38"/>
       <c r="F57" s="39" t="s">
@@ -28758,8 +28754,7 @@
         <v>1</v>
       </c>
       <c r="D58" s="31">
-        <f t="shared" si="55"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58" s="38"/>
       <c r="F58" s="39" t="s">
@@ -29179,7 +29174,7 @@
         <v>0.1</v>
       </c>
       <c r="D59" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>0.1</v>
       </c>
       <c r="E59" s="38"/>
@@ -29600,7 +29595,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="E60" s="38"/>
@@ -30021,7 +30016,7 @@
         <v>1</v>
       </c>
       <c r="D61" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="E61" s="38"/>
@@ -30442,7 +30437,7 @@
         <v>2</v>
       </c>
       <c r="D62" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>2</v>
       </c>
       <c r="E62" s="38"/>
@@ -30863,7 +30858,7 @@
         <v>1</v>
       </c>
       <c r="D63" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="E63" s="38"/>
@@ -31284,7 +31279,7 @@
         <v>1</v>
       </c>
       <c r="D64" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="E64" s="38"/>
@@ -31705,7 +31700,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="31">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="E65" s="38"/>
@@ -32124,7 +32119,7 @@
         <v/>
       </c>
       <c r="D66" s="31" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="E66" s="38"/>
@@ -32541,7 +32536,7 @@
         <v/>
       </c>
       <c r="D67" s="31" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="E67" s="38"/>
@@ -32958,7 +32953,7 @@
         <v/>
       </c>
       <c r="D68" s="31" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="E68" s="38"/>
@@ -33375,7 +33370,7 @@
         <v/>
       </c>
       <c r="D69" s="31" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="E69" s="38"/>

</xml_diff>